<commit_message>
Cleaned code and added material layer with generic data
</commit_message>
<xml_diff>
--- a/docs/Files/ODYM_Config_Vehicle_System.xlsx
+++ b/docs/Files/ODYM_Config_Vehicle_System.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernaag/Box/BATMAN/Coding/Global_model/docs/Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernaag/Box/BATMAN/Coding/V2G_in_EU/docs/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76D60344-0925-3646-8E60-B5606E0B3FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E4FFE7-FA23-CB47-94C2-CD4DEB46F553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="5560" windowWidth="38400" windowHeight="21100" tabRatio="844" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="13740" windowWidth="28800" windowHeight="15860" tabRatio="844" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="5" r:id="rId1"/>
-    <sheet name="Setting_Vehicle_System" sheetId="6" r:id="rId2"/>
+    <sheet name="Setting_V2G_in_EU" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="119">
   <si>
     <t>Description</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Good</t>
-  </si>
-  <si>
     <t>Material</t>
   </si>
   <si>
@@ -213,18 +210,6 @@
     <t>UUID</t>
   </si>
   <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>Regions used</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>region</t>
-  </si>
-  <si>
     <t>Environment</t>
   </si>
   <si>
@@ -252,15 +237,9 @@
     <t>ELV market</t>
   </si>
   <si>
-    <t>Countries</t>
-  </si>
-  <si>
     <t>fernaag</t>
   </si>
   <si>
-    <t>ODYM_Norwegian_Model</t>
-  </si>
-  <si>
     <t>New vehicle market</t>
   </si>
   <si>
@@ -273,12 +252,6 @@
     <t>Second hand dealers are mainly active here</t>
   </si>
   <si>
-    <t>Vehicle_System</t>
-  </si>
-  <si>
-    <t>ODYM_Classifications_Master_Vehicle_System</t>
-  </si>
-  <si>
     <t>Element</t>
   </si>
   <si>
@@ -318,30 +291,9 @@
     <t>Recycling</t>
   </si>
   <si>
-    <t>Segment</t>
-  </si>
-  <si>
-    <t>Weight category of vehicle (curb weight)</t>
-  </si>
-  <si>
     <t>s</t>
   </si>
   <si>
-    <t>Battery_Parts</t>
-  </si>
-  <si>
-    <t>Parts in the battery pack</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>parts</t>
-  </si>
-  <si>
-    <t>segments</t>
-  </si>
-  <si>
     <t>Recycling_Process</t>
   </si>
   <si>
@@ -366,18 +318,12 @@
     <t>scenario</t>
   </si>
   <si>
-    <t>Vehicle stock model for Global fleet</t>
-  </si>
-  <si>
     <t>Size</t>
   </si>
   <si>
     <t>Vehicle size</t>
   </si>
   <si>
-    <t>l</t>
-  </si>
-  <si>
     <t>large</t>
   </si>
   <si>
@@ -423,22 +369,25 @@
     <t>ownership</t>
   </si>
   <si>
-    <t>Day</t>
-  </si>
-  <si>
-    <t>Day time</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>day</t>
-  </si>
-  <si>
     <t>Energy_Storage_Scenarios</t>
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>V2G_in_EU</t>
+  </si>
+  <si>
+    <t>Vehicle stock model for European fleet</t>
+  </si>
+  <si>
+    <t>Drive_train</t>
+  </si>
+  <si>
+    <t>EV_penetration_scenario</t>
+  </si>
+  <si>
+    <t>ODYM_Classifications_Master_V2G</t>
   </si>
 </sst>
 </file>
@@ -1012,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1025,20 +974,20 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" s="36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="8"/>
       <c r="B2" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4" t="s">
-        <v>75</v>
+        <v>114</v>
       </c>
       <c r="G2" s="20"/>
     </row>
@@ -1056,22 +1005,22 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="6" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="G4" s="43"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
       <c r="B5" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="5" t="str">
         <f>E5&amp;D4</f>
-        <v>Setting_Vehicle_System</v>
+        <v>Setting_V2G_in_EU</v>
       </c>
       <c r="E5" s="41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1213,10 +1162,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:K62"/>
+  <dimension ref="B2:K58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1244,10 +1193,10 @@
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C3" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="37"/>
       <c r="F3" s="37"/>
@@ -1262,7 +1211,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="I4" s="20"/>
       <c r="J4" s="20"/>
@@ -1273,7 +1222,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I5" s="20"/>
       <c r="J5" s="9"/>
@@ -1284,7 +1233,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="I6" s="20"/>
       <c r="J6" s="20"/>
@@ -1298,7 +1247,7 @@
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B8" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="26"/>
       <c r="D8" s="26"/>
@@ -1312,13 +1261,13 @@
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C9" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
@@ -1332,7 +1281,7 @@
         <v>6</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>81</v>
+        <v>118</v>
       </c>
       <c r="I10" s="20"/>
       <c r="J10" s="19"/>
@@ -1340,7 +1289,7 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="40" t="s">
         <v>1</v>
@@ -1351,7 +1300,7 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" s="40" t="s">
         <v>1</v>
@@ -1367,11 +1316,11 @@
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B14" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="26"/>
       <c r="D14" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="26"/>
       <c r="F14" s="26"/>
@@ -1398,13 +1347,13 @@
         <v>10</v>
       </c>
       <c r="H15" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="I15" s="42" t="s">
-        <v>51</v>
-      </c>
       <c r="J15" s="35" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="K15" s="20"/>
     </row>
@@ -1413,7 +1362,7 @@
         <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
         <v>11</v>
@@ -1422,620 +1371,528 @@
         <v>11</v>
       </c>
       <c r="G16" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="H16" s="28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C17" s="32" t="s">
-        <v>130</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>131</v>
+        <v>55</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>130</v>
+        <v>11</v>
       </c>
       <c r="G17" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="H17" s="28" t="s">
-        <v>132</v>
+        <v>56</v>
       </c>
       <c r="I17" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C18" s="32" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>86</v>
-      </c>
-      <c r="H18" s="28" t="s">
-        <v>57</v>
+        <v>64</v>
+      </c>
+      <c r="H18" s="28">
+        <v>1</v>
       </c>
       <c r="I18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C19" s="32" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>75</v>
       </c>
       <c r="E19" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="F19" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="G19" t="s">
-        <v>69</v>
-      </c>
-      <c r="H19" s="28">
-        <v>1</v>
-      </c>
-      <c r="I19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="H19" s="28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C20" s="32" t="s">
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="F20" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="G20" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H20" s="28" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="I20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C21" s="32" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D21" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G21" t="s">
-        <v>119</v>
+        <v>64</v>
       </c>
       <c r="H21" s="28" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="I21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C22" s="32" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>106</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
       <c r="F22" t="s">
+        <v>117</v>
+      </c>
+      <c r="G22" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="I22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C23" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="G22" t="s">
-        <v>69</v>
-      </c>
-      <c r="H22" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="I22" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C23" s="32" t="s">
+      <c r="D23" t="s">
         <v>88</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23" t="s">
+        <v>64</v>
+      </c>
+      <c r="H23" s="28" t="s">
         <v>89</v>
-      </c>
-      <c r="E23" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" t="s">
-        <v>88</v>
-      </c>
-      <c r="G23" t="s">
-        <v>69</v>
-      </c>
-      <c r="H23" s="28" t="s">
-        <v>92</v>
       </c>
       <c r="I23" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C24" s="32" t="s">
-        <v>108</v>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C24" s="45" t="s">
+        <v>95</v>
       </c>
       <c r="D24" t="s">
-        <v>124</v>
-      </c>
-      <c r="E24" t="s">
-        <v>108</v>
+        <v>96</v>
+      </c>
+      <c r="E24" s="23" t="s">
+        <v>100</v>
       </c>
       <c r="F24" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="G24" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H24" s="28" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="I24" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C25" s="32" t="s">
-        <v>95</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C25" s="45" t="s">
+        <v>98</v>
       </c>
       <c r="D25" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F25" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G25" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H25" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="I25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C26" s="45" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C26" s="32" t="s">
-        <v>98</v>
-      </c>
       <c r="D26" t="s">
-        <v>99</v>
-      </c>
-      <c r="E26" t="s">
-        <v>13</v>
+        <v>102</v>
       </c>
       <c r="F26" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="G26" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H26" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="I26" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C27" s="32" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C27" s="45" t="s">
+        <v>104</v>
       </c>
       <c r="D27" t="s">
         <v>104</v>
       </c>
-      <c r="E27" t="s">
-        <v>70</v>
-      </c>
       <c r="F27" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G27" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="H27" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="I27" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C28" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" t="s">
+        <v>109</v>
+      </c>
+      <c r="F28" t="s">
+        <v>109</v>
+      </c>
+      <c r="G28" t="s">
+        <v>64</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="I28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C29" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
+        <v>112</v>
+      </c>
+      <c r="F29" t="s">
+        <v>112</v>
+      </c>
+      <c r="G29" t="s">
+        <v>64</v>
+      </c>
+      <c r="H29" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="E28" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="F28" t="s">
-        <v>112</v>
-      </c>
-      <c r="G28" t="s">
+      <c r="I29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="27"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C32" s="33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C33" s="38">
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>59</v>
+      </c>
+      <c r="E33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C34" s="38">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
         <v>69</v>
       </c>
-      <c r="H28" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="I28" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C29" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="D29" t="s">
-        <v>117</v>
-      </c>
-      <c r="E29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" t="s">
-        <v>116</v>
-      </c>
-      <c r="G29" t="s">
-        <v>69</v>
-      </c>
-      <c r="H29" s="28" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C30" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="D30" t="s">
-        <v>120</v>
-      </c>
-      <c r="F30" t="s">
-        <v>120</v>
-      </c>
-      <c r="G30" t="s">
-        <v>69</v>
-      </c>
-      <c r="H30" s="28" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C31" s="45" t="s">
-        <v>122</v>
-      </c>
-      <c r="D31" t="s">
-        <v>122</v>
-      </c>
-      <c r="F31" t="s">
-        <v>122</v>
-      </c>
-      <c r="G31" t="s">
-        <v>69</v>
-      </c>
-      <c r="H31" s="28" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C32" s="45" t="s">
-        <v>127</v>
-      </c>
-      <c r="D32" t="s">
-        <v>127</v>
-      </c>
-      <c r="F32" t="s">
-        <v>127</v>
-      </c>
-      <c r="G32" t="s">
-        <v>69</v>
-      </c>
-      <c r="H32" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="I32" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C33" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="D33" t="s">
-        <v>134</v>
-      </c>
-      <c r="F33" t="s">
-        <v>134</v>
-      </c>
-      <c r="G33" t="s">
-        <v>69</v>
-      </c>
-      <c r="H33" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="I33" t="s">
-        <v>91</v>
+      <c r="E34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B35" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="27"/>
+      <c r="C35" s="34">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C36" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="E36" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="F36" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="G36" s="37"/>
-      <c r="H36" s="37"/>
+      <c r="C36" s="38">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>66</v>
+      </c>
+      <c r="E36" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C37" s="38">
-        <v>0</v>
+      <c r="C37" s="34">
+        <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E37" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C38" s="38">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D38" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="E38" t="s">
-        <v>45</v>
-      </c>
-      <c r="F38" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C39" s="34">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="E39" t="s">
-        <v>45</v>
-      </c>
-      <c r="F39" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C40" s="38">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D40" t="s">
-        <v>71</v>
+        <v>108</v>
       </c>
       <c r="E40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C41" s="34">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D41" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="E41" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C42" s="38">
-        <v>5</v>
-      </c>
-      <c r="D42" t="s">
-        <v>125</v>
-      </c>
-      <c r="E42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C43" s="34">
-        <v>6</v>
-      </c>
-      <c r="D43" t="s">
-        <v>93</v>
-      </c>
-      <c r="E43" t="s">
-        <v>44</v>
-      </c>
+      <c r="B43" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="27"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C44" s="38">
-        <v>7</v>
-      </c>
-      <c r="D44" t="s">
-        <v>126</v>
-      </c>
-      <c r="E44" t="s">
-        <v>44</v>
+      <c r="C44" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="F44" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="G44" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H44" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="I44" s="44" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C45" s="34">
-        <v>8</v>
-      </c>
-      <c r="D45" t="s">
-        <v>94</v>
-      </c>
-      <c r="E45" t="s">
-        <v>44</v>
-      </c>
+      <c r="C45" s="34"/>
+      <c r="F45" s="20"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B46" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="27"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B47" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="27"/>
+      <c r="C47" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C48" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="D48" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="E48" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="F48" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="G48" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="H48" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="I48" s="44" t="s">
-        <v>59</v>
+      <c r="C48" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="E48" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C49" s="34"/>
-      <c r="F49" s="20"/>
+      <c r="D49" s="40"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B50" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C50" s="26"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="26"/>
-      <c r="G50" s="26"/>
-      <c r="H50" s="27"/>
+      <c r="D50" s="40"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C51" t="s">
-        <v>32</v>
-      </c>
+      <c r="D51" s="40"/>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C52" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="D52" s="40" t="s">
-        <v>34</v>
-      </c>
-      <c r="E52" t="s">
-        <v>35</v>
-      </c>
+      <c r="D52" s="40"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D53" s="40"/>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D54" s="40"/>
-    </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D55" s="40"/>
+      <c r="B55" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+      <c r="F55" s="26"/>
+      <c r="G55" s="26"/>
+      <c r="H55" s="27"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D56" s="40"/>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D57" s="40"/>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B59" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="C59" s="26"/>
-      <c r="D59" s="26"/>
-      <c r="E59" s="26"/>
-      <c r="F59" s="26"/>
-      <c r="G59" s="26"/>
-      <c r="H59" s="27"/>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C60" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B62" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="C62" s="26"/>
-      <c r="D62" s="26"/>
-      <c r="E62" s="26"/>
-      <c r="F62" s="26"/>
-      <c r="G62" s="26"/>
-      <c r="H62" s="27"/>
+      <c r="C56" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B58" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="26"/>
+      <c r="F58" s="26"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="27"/>
     </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>

</xml_diff>

<commit_message>
Added V2G ratio parameter file
</commit_message>
<xml_diff>
--- a/docs/Files/ODYM_Config_Vehicle_System.xlsx
+++ b/docs/Files/ODYM_Config_Vehicle_System.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernaag/Box/BATMAN/Coding/V2G_in_EU/docs/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D0FD87-3354-A640-AE9E-1F8B76A97E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E116CD3-1D0C-5342-BB9E-00BD2F97CAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="13980" windowWidth="28800" windowHeight="15860" tabRatio="844" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="13980" windowWidth="28800" windowHeight="17500" tabRatio="844" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="123">
   <si>
     <t>Description</t>
   </si>
@@ -388,6 +388,18 @@
   </si>
   <si>
     <t>[3,6,15,25,27,28]</t>
+  </si>
+  <si>
+    <t>V2G_Scenarios</t>
+  </si>
+  <si>
+    <t>V2G share of vehicle fleet scenarios</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>v2g</t>
   </si>
 </sst>
 </file>
@@ -1162,10 +1174,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:K58"/>
+  <dimension ref="B2:K59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1637,223 +1649,240 @@
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C29" s="45" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D29" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="F29" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="G29" t="s">
         <v>64</v>
       </c>
       <c r="H29" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="I29" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C30" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" t="s">
+        <v>111</v>
+      </c>
+      <c r="F30" t="s">
+        <v>111</v>
+      </c>
+      <c r="G30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H30" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I30" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B31" s="25" t="s">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="27"/>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="27"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C33" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D32" s="30" t="s">
+      <c r="D33" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="E32" s="30" t="s">
+      <c r="E33" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="F32" s="30" t="s">
+      <c r="F33" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37"/>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C33" s="38">
-        <v>0</v>
-      </c>
-      <c r="D33" t="s">
-        <v>59</v>
-      </c>
-      <c r="E33" t="s">
-        <v>59</v>
-      </c>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C34" s="38">
+        <v>0</v>
+      </c>
+      <c r="D34" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C35" s="38">
         <v>1</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>69</v>
-      </c>
-      <c r="E34" t="s">
-        <v>44</v>
-      </c>
-      <c r="F34" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C35" s="34">
-        <v>2</v>
-      </c>
-      <c r="D35" t="s">
-        <v>70</v>
       </c>
       <c r="E35" t="s">
         <v>44</v>
       </c>
       <c r="F35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C36" s="34">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>70</v>
+      </c>
+      <c r="E36" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C36" s="38">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C37" s="38">
         <v>3</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>66</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C37" s="34">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C38" s="34">
         <v>4</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>67</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C38" s="38">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C39" s="38">
         <v>5</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>106</v>
-      </c>
-      <c r="E38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C39" s="34">
-        <v>6</v>
-      </c>
-      <c r="D39" t="s">
-        <v>84</v>
       </c>
       <c r="E39" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C40" s="38">
-        <v>7</v>
+      <c r="C40" s="34">
+        <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="E40" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C41" s="34">
-        <v>8</v>
+      <c r="C41" s="38">
+        <v>7</v>
       </c>
       <c r="D41" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="E41" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B43" s="25" t="s">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C42" s="34">
+        <v>8</v>
+      </c>
+      <c r="D42" t="s">
+        <v>85</v>
+      </c>
+      <c r="E42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B44" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="27"/>
-    </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C44" s="33" t="s">
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="27"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C45" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="D44" s="30" t="s">
+      <c r="D45" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="E44" s="30" t="s">
+      <c r="E45" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="F44" s="30" t="s">
+      <c r="F45" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="G44" s="30" t="s">
+      <c r="G45" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H44" s="30" t="s">
+      <c r="H45" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="I44" s="44" t="s">
+      <c r="I45" s="44" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C45" s="34"/>
-      <c r="F45" s="20"/>
-    </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B46" s="25" t="s">
+      <c r="C46" s="34"/>
+      <c r="F46" s="20"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B47" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
-      <c r="H46" s="27"/>
-    </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C47" t="s">
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="27"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C48" s="34" t="s">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C49" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D48" s="40" t="s">
+      <c r="D49" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E49" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D49" s="40"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D50" s="40"/>
@@ -1867,32 +1896,35 @@
     <row r="53" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D53" s="40"/>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B55" s="25" t="s">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D54" s="40"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B56" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="26"/>
-      <c r="G55" s="26"/>
-      <c r="H55" s="27"/>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C56" t="s">
+      <c r="C56" s="26"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="26"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="27"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C57" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B58" s="25" t="s">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B59" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="C58" s="26"/>
-      <c r="D58" s="26"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="26"/>
-      <c r="G58" s="26"/>
-      <c r="H58" s="27"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="26"/>
+      <c r="G59" s="26"/>
+      <c r="H59" s="27"/>
     </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>

</xml_diff>

<commit_message>
Added capacity for V2G and SLB
</commit_message>
<xml_diff>
--- a/docs/Files/ODYM_Config_Vehicle_System.xlsx
+++ b/docs/Files/ODYM_Config_Vehicle_System.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernaag/Box/BATMAN/Coding/V2G_in_EU/docs/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E116CD3-1D0C-5342-BB9E-00BD2F97CAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBAB1AD-9D04-D04F-B859-01C29C9430A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="13980" windowWidth="28800" windowHeight="17500" tabRatio="844" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2740" yWindow="2880" windowWidth="28800" windowHeight="17500" tabRatio="844" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="124">
   <si>
     <t>Description</t>
   </si>
@@ -400,6 +400,9 @@
   </si>
   <si>
     <t>v2g</t>
+  </si>
+  <si>
+    <t>reuse</t>
   </si>
 </sst>
 </file>
@@ -1176,8 +1179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1626,6 +1629,9 @@
       <c r="H27" s="28" t="s">
         <v>104</v>
       </c>
+      <c r="I27" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C28" s="45" t="s">

</xml_diff>